<commit_message>
add exit confirmation and player message
</commit_message>
<xml_diff>
--- a/bin/Map/map.xlsx
+++ b/bin/Map/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\java\Project\Bomberman2\res\Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7C38A0-A78C-4952-8EF4-3D38B2846CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A629AC3A-0A3A-45E3-98AC-8020F5CAF5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1431,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GG84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EF38" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="EH48" sqref="EH48"/>
+    <sheetView tabSelected="1" topLeftCell="EF1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="EH47" sqref="EH47:EV59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="36.6" x14ac:dyDescent="0.3"/>

</xml_diff>